<commit_message>
Working color by third dimension
</commit_message>
<xml_diff>
--- a/data/bandtest.xlsx
+++ b/data/bandtest.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin.mcgovern\Documents\GitHub\QlikSenseD3ZoomableSunburst\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="11475" windowHeight="5955"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>Parent</t>
   </si>
@@ -91,12 +96,15 @@
   </si>
   <si>
     <t>David Lovering</t>
+  </si>
+  <si>
+    <t>Indicator</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -137,6 +145,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -185,7 +196,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -220,7 +231,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -429,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,7 +452,7 @@
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -451,8 +462,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -462,8 +476,11 @@
       <c r="C2">
         <v>4000</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -473,8 +490,11 @@
       <c r="C3">
         <v>2500</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -484,8 +504,11 @@
       <c r="C4">
         <v>2000</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -495,8 +518,11 @@
       <c r="C5">
         <v>2000</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -506,8 +532,11 @@
       <c r="C6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -517,8 +546,11 @@
       <c r="C7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -528,8 +560,11 @@
       <c r="C8">
         <v>3000</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -539,8 +574,11 @@
       <c r="C9">
         <v>1000</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -550,8 +588,11 @@
       <c r="C10">
         <v>1000</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -561,8 +602,11 @@
       <c r="C11">
         <v>500</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -572,8 +616,11 @@
       <c r="C12">
         <v>1000</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -583,8 +630,11 @@
       <c r="C13">
         <v>500</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -594,8 +644,11 @@
       <c r="C14">
         <v>2000</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -605,8 +658,11 @@
       <c r="C15">
         <v>500</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -616,8 +672,11 @@
       <c r="C16">
         <v>500</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -627,8 +686,11 @@
       <c r="C17">
         <v>500</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -638,8 +700,11 @@
       <c r="C18">
         <v>500</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -649,8 +714,11 @@
       <c r="C19">
         <v>200</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -659,6 +727,9 @@
       </c>
       <c r="C20">
         <v>400</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>